<commit_message>
Prioridades y etapas para comentarios
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="220">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -1197,8 +1197,8 @@
   </sheetPr>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2088,10 +2088,18 @@
       <c r="C37" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
+      <c r="D37" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="H37" s="32"/>
     </row>
     <row r="38" s="33" customFormat="true" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2104,13 +2112,21 @@
       <c r="C38" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
+      <c r="D38" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="H38" s="32"/>
     </row>
-    <row r="39" s="33" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="33" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
         <v>130</v>
       </c>
@@ -2120,10 +2136,18 @@
       <c r="C39" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
+      <c r="D39" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="H39" s="32"/>
     </row>
     <row r="40" s="33" customFormat="true" ht="40.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2136,10 +2160,18 @@
       <c r="C40" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
+      <c r="D40" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H40" s="32"/>
     </row>
     <row r="41" s="33" customFormat="true" ht="39.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2152,10 +2184,18 @@
       <c r="C41" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
+      <c r="D41" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H41" s="32"/>
     </row>
     <row r="42" s="33" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2168,10 +2208,18 @@
       <c r="C42" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
+      <c r="D42" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H42" s="32"/>
     </row>
     <row r="43" s="33" customFormat="true" ht="36.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2184,10 +2232,18 @@
       <c r="C43" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
+      <c r="D43" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="H43" s="32"/>
     </row>
     <row r="44" s="33" customFormat="true" ht="79.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2200,10 +2256,18 @@
       <c r="C44" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
+      <c r="D44" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H44" s="32"/>
     </row>
     <row r="45" s="33" customFormat="true" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2216,10 +2280,18 @@
       <c r="C45" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
+      <c r="D45" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="H45" s="32"/>
     </row>
     <row r="46" s="33" customFormat="true" ht="45.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2232,10 +2304,18 @@
       <c r="C46" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
+      <c r="D46" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H46" s="32"/>
     </row>
     <row r="47" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Se completan todas las prioridades y etapas de las funcionalidades
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="221">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -633,6 +633,9 @@
     <t xml:space="preserve">Desplegar la aplicación en local simulando produción (sin desarrollo para probarla y someterla a tests)</t>
   </si>
   <si>
+    <t xml:space="preserve">Técnico</t>
+  </si>
+  <si>
     <t xml:space="preserve">R57</t>
   </si>
   <si>
@@ -739,7 +742,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -777,19 +780,11 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFDDDDDD"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFDDDDDD"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -889,7 +884,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1102,7 +1097,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,10 +1107,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1195,10 +1186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2318,7 +2309,7 @@
       </c>
       <c r="H46" s="32"/>
     </row>
-    <row r="47" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="39" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>154</v>
       </c>
@@ -2328,13 +2319,21 @@
       <c r="C47" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="D47" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H47" s="38"/>
     </row>
-    <row r="48" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="39" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>157</v>
       </c>
@@ -2344,10 +2343,18 @@
       <c r="C48" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
+      <c r="D48" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H48" s="38"/>
     </row>
     <row r="49" s="39" customFormat="true" ht="40.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2360,13 +2367,21 @@
       <c r="C49" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
+      <c r="D49" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H49" s="38"/>
     </row>
-    <row r="50" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="39" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>163</v>
       </c>
@@ -2376,10 +2391,18 @@
       <c r="C50" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
+      <c r="D50" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H50" s="38"/>
     </row>
     <row r="51" s="39" customFormat="true" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2392,10 +2415,18 @@
       <c r="C51" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
+      <c r="D51" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G51" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H51" s="38"/>
     </row>
     <row r="52" s="39" customFormat="true" ht="40.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2408,13 +2439,21 @@
       <c r="C52" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
+      <c r="D52" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H52" s="38"/>
     </row>
-    <row r="53" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="39" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
         <v>172</v>
       </c>
@@ -2424,13 +2463,21 @@
       <c r="C53" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
+      <c r="D53" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H53" s="38"/>
     </row>
-    <row r="54" s="39" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="39" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
         <v>175</v>
       </c>
@@ -2440,10 +2487,18 @@
       <c r="C54" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
+      <c r="D54" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H54" s="38"/>
     </row>
     <row r="55" s="39" customFormat="true" ht="42.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2456,10 +2511,18 @@
       <c r="C55" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
+      <c r="D55" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H55" s="38"/>
     </row>
     <row r="56" s="39" customFormat="true" ht="186.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2472,10 +2535,18 @@
       <c r="C56" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
+      <c r="D56" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="H56" s="38"/>
     </row>
     <row r="57" s="45" customFormat="true" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2488,203 +2559,319 @@
       <c r="C57" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
+      <c r="D57" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="F57" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="43" t="s">
+        <v>30</v>
+      </c>
       <c r="H57" s="44"/>
     </row>
     <row r="58" s="45" customFormat="true" ht="41.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="D58" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="B58" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="C58" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="F58" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="43" t="s">
+        <v>30</v>
+      </c>
       <c r="H58" s="44"/>
     </row>
     <row r="59" s="45" customFormat="true" ht="39.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
+        <v>193</v>
+      </c>
+      <c r="D59" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="43" t="s">
+        <v>51</v>
+      </c>
       <c r="H59" s="44"/>
     </row>
     <row r="60" s="45" customFormat="true" ht="36.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+        <v>196</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>51</v>
+      </c>
       <c r="H60" s="44"/>
     </row>
     <row r="61" s="45" customFormat="true" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
+        <v>199</v>
+      </c>
+      <c r="D61" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="43" t="s">
+        <v>30</v>
+      </c>
       <c r="H61" s="44"/>
     </row>
     <row r="62" s="50" customFormat="true" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C62" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
+        <v>202</v>
+      </c>
+      <c r="D62" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="H62" s="49"/>
     </row>
     <row r="63" s="50" customFormat="true" ht="40.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C63" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
+        <v>205</v>
+      </c>
+      <c r="D63" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="H63" s="49"/>
     </row>
     <row r="64" s="50" customFormat="true" ht="38.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C64" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="48"/>
+        <v>208</v>
+      </c>
+      <c r="D64" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E64" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="H64" s="49"/>
     </row>
     <row r="65" s="50" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
+        <v>211</v>
+      </c>
+      <c r="D65" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E65" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="H65" s="49"/>
     </row>
     <row r="66" s="50" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>213</v>
-      </c>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
+        <v>214</v>
+      </c>
+      <c r="D66" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="H66" s="49"/>
     </row>
-    <row r="67" s="55" customFormat="true" ht="16.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B67" s="52" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C67" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="54"/>
+        <v>217</v>
+      </c>
+      <c r="D67" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="54" t="s">
+        <v>30</v>
+      </c>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" s="55" customFormat="true" ht="16.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B68" s="52" t="s">
-        <v>218</v>
-      </c>
-      <c r="C68" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="54"/>
+      <c r="C68" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="54" t="s">
+        <v>30</v>
+      </c>
       <c r="H68" s="54"/>
+    </row>
+    <row r="69" s="55" customFormat="true" ht="84.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
+    </row>
+    <row r="70" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D66" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D70" type="list">
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2:E66" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2:E70" type="list">
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2:F66" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2:F70" type="list">
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2:G66" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2:G70" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Se añaden algunas funcionalidades opcionales
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="239">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -720,19 +720,76 @@
     <t xml:space="preserve">R66</t>
   </si>
   <si>
+    <t xml:space="preserve">Exportar estadísticas a PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadísticas como la cantidad de usuarios, cantidad de torrents, descargas totales… podrán ser exportadas a un archivo PDF por un administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R67</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login Google+</t>
   </si>
   <si>
     <t xml:space="preserve">Permite acceder a la aplicación mediante cuenta de Google+</t>
   </si>
   <si>
-    <t xml:space="preserve">R67</t>
+    <t xml:space="preserve">R68</t>
   </si>
   <si>
     <t xml:space="preserve">Login Facebook</t>
   </si>
   <si>
     <t xml:space="preserve">Permite acceder a la aplicación mediante cuenta de Facebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar con API Twitter para crear bot automatizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar con la API de twitter para desarrolladores e integrar con un bot la aplicación de forma que cada hora publique automáticamente un resumen de la actividad:
+- Últimas subidas → enlace y titulos más descargados
+- Lo más descargado del mes → enlace y títulos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar con API Telegram para crear bot automatizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asociar con la API de telegram para crear un bot que publique en un canal de forma automatizada los mismos resúmenes a cada hora.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportar BD en plano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite al administrador exportar la BD completa en texto plano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportar BD en CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permite al administrador exportar la BD completa en formato CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloquear posibles torrents peligrosos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detectar si el archivo que hace referencia el torrent es peligroso o incumple las políticas del sitio.
+En principio esto es difícil de lograr y se filtrará extensiones para bloquear formatos de vídeo y binarios como: mp4,avi,flv,bat,exe…</t>
   </si>
 </sst>
 </file>
@@ -742,7 +799,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -785,6 +842,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFDDDDDD"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -884,7 +947,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1107,6 +1170,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1186,10 +1253,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I74" activeCellId="0" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2680,7 +2747,7 @@
         <v>202</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E62" s="48" t="s">
         <v>12</v>
@@ -2704,7 +2771,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E63" s="48" t="s">
         <v>12</v>
@@ -2728,7 +2795,7 @@
         <v>208</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E64" s="48" t="s">
         <v>12</v>
@@ -2776,7 +2843,7 @@
         <v>214</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E66" s="48" t="s">
         <v>12</v>
@@ -2789,29 +2856,29 @@
       </c>
       <c r="H66" s="49"/>
     </row>
-    <row r="67" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" s="50" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="B67" s="52" t="s">
+      <c r="B67" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="C67" s="53" t="s">
+      <c r="C67" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="D67" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="G67" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="H67" s="54"/>
+      <c r="D67" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G67" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" s="49"/>
     </row>
     <row r="68" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
@@ -2837,41 +2904,165 @@
       </c>
       <c r="H68" s="54"/>
     </row>
-    <row r="69" s="55" customFormat="true" ht="84.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9"/>
-      <c r="B69" s="52"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
+    <row r="69" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="C69" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" s="54" t="s">
+        <v>30</v>
+      </c>
       <c r="H69" s="54"/>
     </row>
-    <row r="70" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9"/>
-      <c r="B70" s="52"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
+    <row r="70" s="55" customFormat="true" ht="84.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B70" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="C70" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="54" t="s">
+        <v>30</v>
+      </c>
       <c r="H70" s="54"/>
+    </row>
+    <row r="71" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B71" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="C71" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="D71" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H71" s="54"/>
+    </row>
+    <row r="72" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="D72" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H72" s="54"/>
+    </row>
+    <row r="73" s="55" customFormat="true" ht="56.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H73" s="54"/>
+    </row>
+    <row r="74" s="55" customFormat="true" ht="85.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="54"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D70" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D74" type="list">
       <formula1>"Mínimo,Importante,Opcional"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2:E70" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2:E74" type="list">
       <formula1>"Técnico,Funcional,Información"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2:F70" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2:F74" type="list">
       <formula1>"Fácil,Media,Difícil"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2:G70" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2:G74" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>